<commit_message>
koodista siivottu turhat kommentoidut osat
</commit_message>
<xml_diff>
--- a/Docs/Excel/eiEsteita.xlsx
+++ b/Docs/Excel/eiEsteita.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7125" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7125" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="eiEsteita8" sheetId="2" r:id="rId1"/>
     <sheet name="eiEsteita" sheetId="1" r:id="rId2"/>
     <sheet name="eiEsteita (2)" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="29">
   <si>
     <t>Lahtotiedosto</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>eiEsteita008.bmp</t>
+  </si>
+  <si>
+    <t>eiEsteita009.bmp</t>
+  </si>
+  <si>
+    <t>eiEsteita0010.bmp</t>
   </si>
 </sst>
 </file>
@@ -585,7 +591,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -597,6 +603,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -779,22 +786,25 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>59</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>167</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>590</c:v>
+                  <c:v>264</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>692</c:v>
+                  <c:v>431</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>741</c:v>
+                  <c:v>959</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>671</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -846,25 +856,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>89</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>333</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>524</c:v>
+                  <c:v>480</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1109</c:v>
+                  <c:v>947</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1569</c:v>
+                  <c:v>1831</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2551</c:v>
+                  <c:v>1472</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5087</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -916,25 +929,28 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>157.74726860521139</c:v>
+                  <c:v>252.39562976833821</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>379.08559179182015</c:v>
+                  <c:v>606.53694686691222</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>704.28029619496488</c:v>
+                  <c:v>1126.848473911944</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1137.1389779277824</c:v>
+                  <c:v>1819.4223646844518</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1680.5966674922679</c:v>
+                  <c:v>2688.9546679876289</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2337.0440964025925</c:v>
+                  <c:v>3739.2705542441481</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3108.4990562424732</c:v>
+                  <c:v>4973.5984899879568</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6394.7320235020288</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -951,11 +967,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="416275992"/>
-        <c:axId val="416282264"/>
+        <c:axId val="409704672"/>
+        <c:axId val="409704280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="416275992"/>
+        <c:axId val="409704672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -997,7 +1013,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="416282264"/>
+        <c:crossAx val="409704280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1005,7 +1021,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="416282264"/>
+        <c:axId val="409704280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1056,7 +1072,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="416275992"/>
+        <c:crossAx val="409704672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1261,22 +1277,25 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>298</c:v>
+                  <c:v>282</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>437</c:v>
+                  <c:v>312</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1328,25 +1347,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>70</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>140</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>220</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>380</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>760</c:v>
+                  <c:v>602</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1267</c:v>
+                  <c:v>777</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1122</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1418,6 +1440,9 @@
                 <c:pt idx="6">
                   <c:v>1865.0994337454836</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>2398.0245088132606</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1433,11 +1458,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="424746088"/>
-        <c:axId val="424742952"/>
+        <c:axId val="409703104"/>
+        <c:axId val="410962896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="424746088"/>
+        <c:axId val="409703104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1479,7 +1504,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424742952"/>
+        <c:crossAx val="410962896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1487,7 +1512,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="424742952"/>
+        <c:axId val="410962896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1538,7 +1563,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="424746088"/>
+        <c:crossAx val="409703104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1924,11 +1949,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="331664616"/>
-        <c:axId val="331665008"/>
+        <c:axId val="410963288"/>
+        <c:axId val="410963680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="331664616"/>
+        <c:axId val="410963288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1970,7 +1995,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="331665008"/>
+        <c:crossAx val="410963680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1978,7 +2003,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="331665008"/>
+        <c:axId val="410963680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2029,7 +2054,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="331664616"/>
+        <c:crossAx val="410963288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2415,11 +2440,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="331665400"/>
-        <c:axId val="331665792"/>
+        <c:axId val="410964464"/>
+        <c:axId val="410964856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="331665400"/>
+        <c:axId val="410964464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2461,7 +2486,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="331665792"/>
+        <c:crossAx val="410964856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2469,7 +2494,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="331665792"/>
+        <c:axId val="410964856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2520,7 +2545,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="331665400"/>
+        <c:crossAx val="410964464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5467,8 +5492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5494,26 +5519,26 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="I1" s="5"/>
+      <c r="J1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="5"/>
       <c r="O1">
-        <v>2.5000000000000001E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="P1">
         <v>1.4999999999999999E-4</v>
@@ -5567,37 +5592,37 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>300</v>
+      </c>
+      <c r="C3" s="1">
+        <v>200</v>
+      </c>
+      <c r="D3" s="1">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1">
+        <v>7</v>
+      </c>
+      <c r="H3" s="1">
         <v>10</v>
       </c>
-      <c r="B3" s="2">
-        <v>300</v>
-      </c>
-      <c r="C3" s="2">
-        <v>200</v>
-      </c>
-      <c r="D3" s="2">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2">
-        <v>89</v>
-      </c>
-      <c r="G3" s="2">
-        <v>7</v>
-      </c>
-      <c r="H3" s="2">
-        <v>10</v>
-      </c>
-      <c r="I3" s="2">
-        <v>30</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="I3" s="1">
+        <v>20</v>
+      </c>
+      <c r="J3" s="1">
         <v>170</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="1">
         <v>170</v>
       </c>
       <c r="L3" s="2">
@@ -5614,45 +5639,45 @@
       </c>
       <c r="O3" s="4">
         <f>$N3*O$1</f>
-        <v>157.74726860521139</v>
+        <v>252.39562976833821</v>
       </c>
       <c r="P3" s="4">
-        <f t="shared" ref="P3:P9" si="0">$N3*P$1</f>
+        <f t="shared" ref="P3:P10" si="0">$N3*P$1</f>
         <v>94.648361163126808</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1">
         <v>450</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>300</v>
       </c>
-      <c r="D4" s="2">
-        <v>40</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="D4" s="1">
+        <v>27</v>
+      </c>
+      <c r="E4" s="1">
         <v>7</v>
       </c>
-      <c r="F4" s="2">
-        <v>82</v>
-      </c>
-      <c r="G4" s="2">
+      <c r="F4" s="1">
+        <v>78</v>
+      </c>
+      <c r="G4" s="1">
         <v>7</v>
       </c>
-      <c r="H4" s="2">
-        <v>20</v>
-      </c>
-      <c r="I4" s="2">
-        <v>70</v>
-      </c>
-      <c r="J4" s="2">
+      <c r="H4" s="1">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1">
+        <v>50</v>
+      </c>
+      <c r="J4" s="1">
         <v>255</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <v>255</v>
       </c>
       <c r="L4" s="2">
@@ -5668,8 +5693,8 @@
         <v>1516342.3671672805</v>
       </c>
       <c r="O4" s="4">
-        <f t="shared" ref="O4:P9" si="4">$N4*O$1</f>
-        <v>379.08559179182015</v>
+        <f t="shared" ref="O4:O10" si="4">$N4*O$1</f>
+        <v>606.53694686691222</v>
       </c>
       <c r="P4" s="4">
         <f t="shared" si="0"/>
@@ -5677,37 +5702,37 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1">
         <v>600</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>400</v>
       </c>
-      <c r="D5" s="2">
-        <v>59</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="D5" s="1">
+        <v>98</v>
+      </c>
+      <c r="E5" s="1">
         <v>7</v>
       </c>
-      <c r="F5" s="2">
-        <v>333</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="F5" s="1">
+        <v>218</v>
+      </c>
+      <c r="G5" s="1">
         <v>7</v>
       </c>
-      <c r="H5" s="2">
-        <v>40</v>
-      </c>
-      <c r="I5" s="2">
-        <v>140</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="H5" s="1">
+        <v>30</v>
+      </c>
+      <c r="I5" s="1">
+        <v>110</v>
+      </c>
+      <c r="J5" s="1">
         <v>340</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>340</v>
       </c>
       <c r="L5" s="2">
@@ -5724,7 +5749,7 @@
       </c>
       <c r="O5" s="4">
         <f t="shared" si="4"/>
-        <v>704.28029619496488</v>
+        <v>1126.848473911944</v>
       </c>
       <c r="P5" s="4">
         <f t="shared" si="0"/>
@@ -5732,37 +5757,37 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1">
         <v>750</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>500</v>
       </c>
-      <c r="D6" s="2">
-        <v>167</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D6" s="1">
+        <v>79</v>
+      </c>
+      <c r="E6" s="1">
         <v>7</v>
       </c>
-      <c r="F6" s="2">
-        <v>524</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="F6" s="1">
+        <v>480</v>
+      </c>
+      <c r="G6" s="1">
         <v>7</v>
       </c>
-      <c r="H6" s="2">
-        <v>80</v>
-      </c>
-      <c r="I6" s="2">
-        <v>220</v>
-      </c>
-      <c r="J6" s="2">
+      <c r="H6" s="1">
+        <v>50</v>
+      </c>
+      <c r="I6" s="1">
+        <v>180</v>
+      </c>
+      <c r="J6" s="1">
         <v>425</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="1">
         <v>425</v>
       </c>
       <c r="L6" s="2">
@@ -5779,7 +5804,7 @@
       </c>
       <c r="O6" s="4">
         <f t="shared" si="4"/>
-        <v>1137.1389779277824</v>
+        <v>1819.4223646844518</v>
       </c>
       <c r="P6" s="4">
         <f t="shared" si="0"/>
@@ -5787,37 +5812,37 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1">
         <v>900</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>600</v>
       </c>
-      <c r="D7" s="2">
-        <v>590</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D7" s="1">
+        <v>264</v>
+      </c>
+      <c r="E7" s="1">
         <v>7</v>
       </c>
-      <c r="F7" s="2">
-        <v>1109</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="F7" s="1">
+        <v>947</v>
+      </c>
+      <c r="G7" s="1">
         <v>7</v>
       </c>
-      <c r="H7" s="2">
-        <v>100</v>
-      </c>
-      <c r="I7" s="2">
-        <v>380</v>
-      </c>
-      <c r="J7" s="2">
+      <c r="H7" s="1">
+        <v>70</v>
+      </c>
+      <c r="I7" s="1">
+        <v>512</v>
+      </c>
+      <c r="J7" s="1">
         <v>510</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="1">
         <v>510</v>
       </c>
       <c r="L7" s="2">
@@ -5834,7 +5859,7 @@
       </c>
       <c r="O7" s="4">
         <f t="shared" si="4"/>
-        <v>1680.5966674922679</v>
+        <v>2688.9546679876289</v>
       </c>
       <c r="P7" s="4">
         <f t="shared" si="0"/>
@@ -5842,37 +5867,37 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1">
         <v>1050</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>700</v>
       </c>
-      <c r="D8" s="2">
-        <v>692</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="D8" s="1">
+        <v>431</v>
+      </c>
+      <c r="E8" s="1">
         <v>7</v>
       </c>
-      <c r="F8" s="2">
-        <v>1569</v>
-      </c>
-      <c r="G8" s="2">
+      <c r="F8" s="1">
+        <v>1831</v>
+      </c>
+      <c r="G8" s="1">
         <v>7</v>
       </c>
-      <c r="H8" s="2">
-        <v>298</v>
-      </c>
-      <c r="I8" s="2">
-        <v>760</v>
-      </c>
-      <c r="J8" s="2">
+      <c r="H8" s="1">
+        <v>282</v>
+      </c>
+      <c r="I8" s="1">
+        <v>602</v>
+      </c>
+      <c r="J8" s="1">
         <v>595</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="1">
         <v>595</v>
       </c>
       <c r="L8" s="2">
@@ -5889,7 +5914,7 @@
       </c>
       <c r="O8" s="4">
         <f t="shared" si="4"/>
-        <v>2337.0440964025925</v>
+        <v>3739.2705542441481</v>
       </c>
       <c r="P8" s="4">
         <f t="shared" si="0"/>
@@ -5897,37 +5922,37 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1">
         <v>1200</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>800</v>
       </c>
-      <c r="D9" s="2">
-        <v>741</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="D9" s="1">
+        <v>959</v>
+      </c>
+      <c r="E9" s="1">
         <v>7</v>
       </c>
-      <c r="F9" s="2">
-        <v>2551</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="F9" s="1">
+        <v>1472</v>
+      </c>
+      <c r="G9" s="1">
         <v>7</v>
       </c>
-      <c r="H9" s="2">
-        <v>437</v>
-      </c>
-      <c r="I9" s="2">
-        <v>1267</v>
-      </c>
-      <c r="J9" s="2">
+      <c r="H9" s="1">
+        <v>312</v>
+      </c>
+      <c r="I9" s="1">
+        <v>777</v>
+      </c>
+      <c r="J9" s="1">
         <v>680</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="1">
         <v>680</v>
       </c>
       <c r="L9" s="2">
@@ -5944,7 +5969,7 @@
       </c>
       <c r="O9" s="4">
         <f t="shared" si="4"/>
-        <v>3108.4990562424732</v>
+        <v>4973.5984899879568</v>
       </c>
       <c r="P9" s="4">
         <f t="shared" si="0"/>
@@ -5952,21 +5977,59 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1350</v>
+      </c>
+      <c r="C10" s="1">
+        <v>900</v>
+      </c>
+      <c r="D10" s="1">
+        <v>671</v>
+      </c>
+      <c r="E10" s="1">
+        <v>7</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5087</v>
+      </c>
+      <c r="G10" s="1">
+        <v>7</v>
+      </c>
+      <c r="H10" s="1">
+        <v>492</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1122</v>
+      </c>
+      <c r="J10" s="1">
+        <v>765</v>
+      </c>
+      <c r="K10" s="1">
+        <v>765</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" ref="L10" si="5">B10*C10</f>
+        <v>1215000</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" ref="M10" si="6">(B10-1)*(C10-1)*2+(B10-1)+(C10-1)</f>
+        <v>2427750</v>
+      </c>
+      <c r="N10" s="4">
+        <f t="shared" ref="N10" si="7">L10+M10*LOG(L10)</f>
+        <v>15986830.058755072</v>
+      </c>
+      <c r="O10" s="4">
+        <f t="shared" si="4"/>
+        <v>6394.7320235020288</v>
+      </c>
+      <c r="P10" s="4">
+        <f t="shared" si="0"/>
+        <v>2398.0245088132606</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5984,7 +6047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L10" sqref="L10:P10"/>
     </sheetView>
   </sheetViews>
@@ -6011,24 +6074,24 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="I1" s="5"/>
+      <c r="J1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="5"/>
       <c r="O1">
         <v>2.5000000000000001E-4</v>
       </c>
@@ -6185,7 +6248,7 @@
         <v>1516342.3671672805</v>
       </c>
       <c r="O4" s="4">
-        <f t="shared" ref="O4:P10" si="4">$N4*O$1</f>
+        <f t="shared" ref="O4:O10" si="4">$N4*O$1</f>
         <v>379.08559179182015</v>
       </c>
       <c r="P4" s="4">

</xml_diff>